<commit_message>
revised assessment details column
</commit_message>
<xml_diff>
--- a/doc/Mass_Upload_Template .xlsx
+++ b/doc/Mass_Upload_Template .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmattioli\Projects\XNAT-Interact\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5A637B-F335-4830-BFDC-EF7AD2F5D251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC40803-7D84-4D4E-A7C3-080D7590C856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5610" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{14F289B2-7387-4F9E-AE69-8F29271F5EC7}"/>
+    <workbookView xWindow="-28920" yWindow="-5610" windowWidth="29040" windowHeight="15720" xr2:uid="{14F289B2-7387-4F9E-AE69-8F29271F5EC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    If none/unknown, leave blank. Otherwise, list the full name of the assessment</t>
+    If unknown, leave blank.</t>
       </text>
     </comment>
     <comment ref="V1" authorId="8" shapeId="0" xr:uid="{B006CA48-F70C-4C63-B71C-CBE061597E6A}">
@@ -134,7 +134,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Free form -- date of assessment; score; etc.</t>
+    Free form -- full name, date of assessment; score, etc.</t>
       </text>
     </comment>
     <comment ref="X1" authorId="10" shapeId="0" xr:uid="{A994F9F3-7C93-4F54-A895-B5CF0D28CB44}">
@@ -261,11 +261,6 @@
 HawkID</t>
   </si>
   <si>
-    <t>Additional
-Assessment
-Details</t>
-  </si>
-  <si>
     <t>Name/
 Type of
 Storage
@@ -607,6 +602,10 @@
   <si>
     <t>Case Name
 [Optional]</t>
+  </si>
+  <si>
+    <t>Assessment
+Details</t>
   </si>
 </sst>
 </file>
@@ -1195,13 +1194,13 @@
     <text>BMI, pre-existing conditions, etc.</text>
   </threadedComment>
   <threadedComment ref="U1" dT="2024-09-10T17:20:29.95" personId="{09F1D53E-6429-4942-B85E-DCF0210217E4}" id="{85C4F7FB-29AA-45A2-90C2-21AAE02E4262}">
-    <text>If none/unknown, leave blank. Otherwise, list the full name of the assessment</text>
+    <text>If unknown, leave blank.</text>
   </threadedComment>
   <threadedComment ref="V1" dT="2024-09-10T17:20:57.83" personId="{09F1D53E-6429-4942-B85E-DCF0210217E4}" id="{B006CA48-F70C-4C63-B71C-CBE061597E6A}">
     <text>Leave blank if none/unknown</text>
   </threadedComment>
   <threadedComment ref="W1" dT="2024-09-10T17:21:30.94" personId="{09F1D53E-6429-4942-B85E-DCF0210217E4}" id="{7EDC5708-658D-4C64-87EF-AAF708C58B95}">
-    <text>Free form -- date of assessment; score; etc.</text>
+    <text>Free form -- full name, date of assessment; score, etc.</text>
   </threadedComment>
   <threadedComment ref="X1" dT="2024-09-10T17:22:09.14" personId="{09F1D53E-6429-4942-B85E-DCF0210217E4}" id="{A994F9F3-7C93-4F54-A895-B5CF0D28CB44}">
     <text>e.g., usb drive; EPIC; etc</text>
@@ -1219,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74064FA1-C69E-4BD8-8AA5-5C0A1EF477B5}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1255,7 +1254,7 @@
   <sheetData>
     <row r="1" spans="1:26" s="13" customFormat="1" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>2</v>
@@ -1303,7 +1302,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>15</v>
@@ -1321,53 +1320,53 @@
         <v>19</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Z1" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="23" t="s">
+      <c r="E2" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="26" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>32</v>
       </c>
       <c r="H2" s="26"/>
       <c r="I2" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N2" s="27"/>
       <c r="O2" s="27"/>
@@ -1375,21 +1374,21 @@
         <v>2</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R2" s="24"/>
       <c r="S2" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
       <c r="V2" s="24"/>
       <c r="W2" s="24"/>
       <c r="X2" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y2" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z2" s="24"/>
     </row>
@@ -3747,7 +3746,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{D26AEC6A-0B02-4D3B-8E70-37A3CD9708A8}">
       <formula1>40179</formula1>
     </dataValidation>
@@ -3758,6 +3757,9 @@
     <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:H1048576" xr:uid="{555A59A2-F056-4FDC-B82B-8BD91AD52720}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{764DD80B-2C61-43B5-8603-9A514DA7594D}">
+      <formula1>"Y, N, Unknown"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3818,7 +3820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DEE2E1-DFE1-4A7A-9865-D4F1FA133515}">
   <dimension ref="A1:XFC100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -3837,155 +3839,155 @@
   <sheetData>
     <row r="1" spans="1:7" s="14" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>39</v>
-      </c>
       <c r="G1" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
       <c r="D7" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3993,11 +3995,11 @@
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4005,11 +4007,11 @@
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4017,11 +4019,11 @@
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4029,11 +4031,11 @@
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4041,11 +4043,11 @@
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4053,11 +4055,11 @@
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4065,11 +4067,11 @@
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4077,11 +4079,11 @@
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4089,11 +4091,11 @@
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,11 +4103,11 @@
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4113,11 +4115,11 @@
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4125,11 +4127,11 @@
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4137,11 +4139,11 @@
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4149,11 +4151,11 @@
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,11 +4163,11 @@
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4173,11 +4175,11 @@
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4185,11 +4187,11 @@
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4197,11 +4199,11 @@
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4209,11 +4211,11 @@
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,11 +4223,11 @@
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4233,11 +4235,11 @@
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4247,7 +4249,7 @@
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4257,7 +4259,7 @@
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4267,7 +4269,7 @@
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4277,7 +4279,7 @@
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4287,7 +4289,7 @@
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4297,7 +4299,7 @@
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4307,7 +4309,7 @@
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4317,7 +4319,7 @@
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4327,7 +4329,7 @@
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4337,7 +4339,7 @@
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -4347,7 +4349,7 @@
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4357,7 +4359,7 @@
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -4367,7 +4369,7 @@
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4377,7 +4379,7 @@
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25"/>

</xml_diff>